<commit_message>
Excel report templates in spanish and metric units.
</commit_message>
<xml_diff>
--- a/templates/export/summary.xlsx
+++ b/templates/export/summary.xlsx
@@ -60,37 +60,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
-    <t xml:space="preserve">Report type:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period:</t>
+    <t xml:space="preserve">Tipo de reporte:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Periodo:</t>
   </si>
   <si>
     <t xml:space="preserve">${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
   </si>
   <si>
-    <t xml:space="preserve">Device</t>
+    <t xml:space="preserve">Dispositivo</t>
   </si>
   <si>
     <t xml:space="preserve">Object</t>
   </si>
   <si>
-    <t xml:space="preserve">Distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Top speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engine Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spent Fuel</t>
+    <t xml:space="preserve">Distancia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad máxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad promedio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horas de motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combustible consumido</t>
   </si>
   <si>
     <t xml:space="preserve">${summary.deviceName}</t>
@@ -99,10 +99,10 @@
     <t xml:space="preserve">${distanceUnit.equals("mi") ? "".format("%.1f mi", summary.distance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", summary.distance * 0.000539957) : "".format("%.1f km", summary.distance * 0.001)}</t>
   </si>
   <si>
-    <t xml:space="preserve">${speedUnit.equals("kmh") ? "".format("%.1f km/h", summary.maxSpeed * 1.852) : speedUnit.equals("mph") ? "".format("%.1f mph", summary.maxSpeed * 1.15078) : "".format("%.1f kn", summary.maxSpeed)}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${speedUnit.equals("kmh") ? "".format("%.1f km/h", summary.averageSpeed * 1.852) : speedUnit.equals("mph") ? "".format("%.1f mph", summary.averageSpeed * 1.15078) : "".format("%.1f kn", summary.averageSpeed)}</t>
+    <t xml:space="preserve">${speedUnit.equals("kmh") ? "".format("%.1f km/h", summary.maxSpeed) : speedUnit.equals("mph") ? "".format("%.1f mph", summary.maxSpeed * 0.621371) : "".format("%.1f kn", summary.maxSpeed*0.539957)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${speedUnit.equals("kmh") ? "".format("%.1f km/h", summary.averageSpeed) : speedUnit.equals("mph") ? "".format("%.1f mph", summary.averageSpeed *0.621371) : "".format("%.1f kn", summary.averageSpeed*0.539957)}</t>
   </si>
   <si>
     <t xml:space="preserve">${summary.engineHours/86400000.0}</t>
@@ -405,9 +405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>323640</xdr:colOff>
+      <xdr:colOff>322560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -417,7 +417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10701360" cy="9524520"/>
+          <a:ext cx="10697760" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -450,9 +450,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>323640</xdr:colOff>
+      <xdr:colOff>322560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -462,7 +462,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10701360" cy="9524520"/>
+          <a:ext cx="10697760" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -496,17 +496,17 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.68367346938776"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +517,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -599,7 +599,7 @@
       <c r="F7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>